<commit_message>
v1 e v2 a funcionar
</commit_message>
<xml_diff>
--- a/project2/report/dados/Tempos.xlsx
+++ b/project2/report/dados/Tempos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joana\Documents\Escola\Engenharia Informática\5ºAno\1ºSemestre\Computação de Alto Desempenho\Projetos\ProjetosCAD\project2\report\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6D7ACB-382E-436A-9FEF-7644F6F9D9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28804DBC-6C8B-4E05-AA16-EBCFFFC035F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{6046D603-8F72-4B98-AF66-112E83401992}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6046D603-8F72-4B98-AF66-112E83401992}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
@@ -106,8 +106,8 @@
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939A7B2A-1526-4CDB-84A6-7D06D3F4B75A}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -430,7 +430,7 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25">
+    <row r="1" spans="1:8" ht="26.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -452,8 +452,11 @@
       <c r="G1" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>144.62270000000001</v>
       </c>
@@ -469,8 +472,17 @@
       <c r="E2" s="2">
         <v>10.235559</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2">
+        <v>10.797729</v>
+      </c>
+      <c r="G2">
+        <v>8.6426719999999992</v>
+      </c>
+      <c r="H2">
+        <v>7.5365580000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>144.83444399999999</v>
       </c>
@@ -486,8 +498,17 @@
       <c r="E3" s="2">
         <v>10.309411000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3">
+        <v>10.795088</v>
+      </c>
+      <c r="G3">
+        <v>8.5726130000000005</v>
+      </c>
+      <c r="H3">
+        <v>7.9841420000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>144.65252899999999</v>
       </c>
@@ -503,8 +524,17 @@
       <c r="E4" s="2">
         <v>10.159136999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4">
+        <v>10.769329000000001</v>
+      </c>
+      <c r="G4">
+        <v>8.4481959999999994</v>
+      </c>
+      <c r="H4">
+        <v>7.4888880000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>144.67921999999999</v>
       </c>
@@ -520,8 +550,17 @@
       <c r="E5" s="2">
         <v>10.296944</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5">
+        <v>10.767128</v>
+      </c>
+      <c r="G5">
+        <v>8.5706430000000005</v>
+      </c>
+      <c r="H5">
+        <v>7.4482249999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>144.83310700000001</v>
       </c>
@@ -537,8 +576,17 @@
       <c r="E6" s="2">
         <v>10.244574999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6">
+        <v>10.945178</v>
+      </c>
+      <c r="G6">
+        <v>8.5990020000000005</v>
+      </c>
+      <c r="H6">
+        <v>7.155856</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>144.72927200000001</v>
       </c>
@@ -554,8 +602,17 @@
       <c r="E7" s="2">
         <v>10.225892</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="F7">
+        <v>10.794335</v>
+      </c>
+      <c r="G7">
+        <v>8.5672300000000003</v>
+      </c>
+      <c r="H7">
+        <v>7.1304379999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>144.67749499999999</v>
       </c>
@@ -571,8 +628,17 @@
       <c r="E8" s="2">
         <v>10.169905999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="F8">
+        <v>10.849694</v>
+      </c>
+      <c r="G8">
+        <v>8.5589980000000008</v>
+      </c>
+      <c r="H8">
+        <v>7.227595</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>144.75439600000001</v>
       </c>
@@ -588,8 +654,17 @@
       <c r="E9" s="2">
         <v>10.231118</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9">
+        <v>10.903616</v>
+      </c>
+      <c r="G9">
+        <v>8.4926879999999993</v>
+      </c>
+      <c r="H9">
+        <v>7.361364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>144.66944899999999</v>
       </c>
@@ -605,8 +680,17 @@
       <c r="E10" s="2">
         <v>10.259917</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="F10">
+        <v>10.83319</v>
+      </c>
+      <c r="G10">
+        <v>8.610989</v>
+      </c>
+      <c r="H10">
+        <v>7.5399700000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>144.93324000000001</v>
       </c>
@@ -622,8 +706,17 @@
       <c r="E11" s="2">
         <v>10.153103</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="18">
+      <c r="F11">
+        <v>10.864084</v>
+      </c>
+      <c r="G11">
+        <v>8.6026410000000002</v>
+      </c>
+      <c r="H11">
+        <v>7.6326910000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18">
       <c r="A12" s="3">
         <f t="shared" ref="A12:C12" si="0">AVERAGE(A2:A11)</f>
         <v>144.73858520000002</v>
@@ -644,13 +737,17 @@
         <f>AVERAGE(E2:E11)</f>
         <v>10.2285562</v>
       </c>
-      <c r="F12" s="3" t="e">
-        <f t="shared" ref="F12:G12" si="1">AVERAGE(F2:F11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G12" s="3" t="e">
+      <c r="F12" s="3">
+        <f t="shared" ref="F12:H12" si="1">AVERAGE(F2:F11)</f>
+        <v>10.831937100000001</v>
+      </c>
+      <c r="G12" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>8.5665672000000015</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="1"/>
+        <v>7.4505726999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>